<commit_message>
alive again (added all hospitals to catchment area calculations)
</commit_message>
<xml_diff>
--- a/catchment_areas_over_time.xlsx
+++ b/catchment_areas_over_time.xlsx
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,21 +42,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO7"/>
+  <dimension ref="A1:AO11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,207 +422,207 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>Hospital</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>2023-10-01 to 2023-10-15</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>2023-10-15 to 2023-10-29</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>2023-10-29 to 2023-11-12</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>2023-11-12 to 2023-11-26</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>2023-11-26 to 2023-12-10</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>2023-12-10 to 2023-12-24</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>2023-12-24 to 2024-01-07</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>2024-01-07 to 2024-01-21</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>2024-01-21 to 2024-02-04</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>2024-02-04 to 2024-02-18</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>2024-02-18 to 2024-03-03</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>2024-03-03 to 2024-03-17</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>2024-03-17 to 2024-03-31</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>2024-03-31 to 2024-04-14</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>2024-04-14 to 2024-04-28</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>2024-04-28 to 2024-05-12</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>2024-05-12 to 2024-05-26</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>2024-05-26 to 2024-06-09</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" t="inlineStr">
         <is>
           <t>2024-06-09 to 2024-06-23</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
         <is>
           <t>2024-06-23 to 2024-07-07</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" t="inlineStr">
         <is>
           <t>2024-07-07 to 2024-07-21</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" t="inlineStr">
         <is>
           <t>2024-07-21 to 2024-08-04</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" t="inlineStr">
         <is>
           <t>2024-08-04 to 2024-08-18</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" t="inlineStr">
         <is>
           <t>2024-08-18 to 2024-09-01</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" t="inlineStr">
         <is>
           <t>2024-09-01 to 2024-09-15</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>2024-09-15 to 2024-09-29</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>2024-09-29 to 2024-10-13</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>2024-10-13 to 2024-10-27</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>2024-10-27 to 2024-11-10</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>2024-11-10 to 2024-11-24</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>2024-11-24 to 2024-12-08</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AG1" t="inlineStr">
         <is>
           <t>2024-12-08 to 2024-12-22</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AH1" t="inlineStr">
         <is>
           <t>2024-12-22 to 2025-01-05</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AI1" t="inlineStr">
         <is>
           <t>2025-01-05 to 2025-01-19</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AJ1" t="inlineStr">
         <is>
           <t>2025-01-19 to 2025-02-02</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AK1" t="inlineStr">
         <is>
           <t>2025-02-02 to 2025-02-16</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="AL1" t="inlineStr">
         <is>
           <t>2025-02-16 to 2025-03-02</t>
         </is>
       </c>
-      <c r="AM1" s="1" t="inlineStr">
+      <c r="AM1" t="inlineStr">
         <is>
           <t>2025-03-02 to 2025-03-16</t>
         </is>
       </c>
-      <c r="AN1" s="1" t="inlineStr">
+      <c r="AN1" t="inlineStr">
         <is>
           <t>2025-03-16 to 2025-03-19</t>
         </is>
       </c>
-      <c r="AO1" s="1" t="inlineStr">
+      <c r="AO1" t="inlineStr">
         <is>
           <t>Average</t>
         </is>
@@ -647,986 +635,1646 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="C2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="D2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="E2" t="n">
-        <v>37.87426464575326</v>
+        <v>23.43202023968979</v>
       </c>
       <c r="F2" t="n">
-        <v>41.31737961354902</v>
+        <v>25.56220389784341</v>
       </c>
       <c r="G2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="H2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="I2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="J2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="K2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="L2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="M2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="N2" t="n">
-        <v>3.443114967795751</v>
+        <v>2.130183658153618</v>
       </c>
       <c r="O2" t="n">
-        <v>44.76049458134477</v>
+        <v>27.69238755599703</v>
       </c>
       <c r="P2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="Q2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="R2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="S2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="T2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="U2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="V2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="W2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="X2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="Y2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="Z2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AA2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AB2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AC2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AD2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AE2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AF2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AG2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AH2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AI2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AJ2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AK2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AL2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AM2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AN2" t="n">
-        <v>48.20360954914052</v>
+        <v>29.82257121415065</v>
       </c>
       <c r="AO2" t="n">
-        <v>46.52619456482977</v>
+        <v>28.78478943197325</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>11.05%</t>
+          <t>6.84%</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>12.06%</t>
+          <t>7.46%</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>1.00%</t>
+          <t>0.62%</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>13.06%</t>
+          <t>8.08%</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AL3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AM3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AN3" t="inlineStr">
         <is>
-          <t>14.07%</t>
+          <t>8.70%</t>
         </is>
       </c>
       <c r="AO3" t="inlineStr">
         <is>
-          <t>13.58%</t>
+          <t>8.40%</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>European Hospital</t>
+          <t>Al-Quds Hospital</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="C4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="D4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="E4" t="n">
-        <v>46.43282981975963</v>
+        <v>26.63565617394064</v>
       </c>
       <c r="F4" t="n">
-        <v>50.6539961670105</v>
+        <v>29.0570794624807</v>
       </c>
       <c r="G4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="H4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="I4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="J4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="K4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="L4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="M4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="N4" t="n">
-        <v>59.0612968836448</v>
+        <v>49.58845710065333</v>
       </c>
       <c r="O4" t="n">
-        <v>59.093634093984</v>
+        <v>35.10673612118332</v>
       </c>
       <c r="P4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="Q4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="R4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="S4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="T4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="U4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="V4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="W4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="X4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="Y4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="Z4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AA4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AB4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AC4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AD4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AE4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AF4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AG4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AH4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AI4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AJ4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AK4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AL4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AM4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AN4" t="n">
-        <v>59.09632886151226</v>
+        <v>33.89992603956082</v>
       </c>
       <c r="AO4" t="n">
-        <v>58.55418633634175</v>
+        <v>34.02270103186888</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>13.55%</t>
+          <t>7.77%</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>14.78%</t>
+          <t>8.48%</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>17.24%</t>
+          <t>14.47%</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>10.25%</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AL5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AN5" t="inlineStr">
         <is>
-          <t>17.25%</t>
+          <t>9.89%</t>
         </is>
       </c>
       <c r="AO5" t="inlineStr">
         <is>
-          <t>17.09%</t>
+          <t>9.93%</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Nasser Hospital</t>
+          <t>European Hospital</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="C6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="D6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="E6" t="n">
-        <v>43.85873461215358</v>
+        <v>41.31907113094489</v>
       </c>
       <c r="F6" t="n">
-        <v>47.84589230416755</v>
+        <v>45.07535032466715</v>
       </c>
       <c r="G6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="H6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="I6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="J6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="K6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="L6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="M6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="N6" t="n">
-        <v>55.85511288298441</v>
+        <v>52.5875770377351</v>
       </c>
       <c r="O6" t="n">
-        <v>55.82289270317924</v>
+        <v>52.58788319869809</v>
       </c>
       <c r="P6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="Q6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="R6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="S6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="T6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="U6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="V6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="W6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="X6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="Y6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="Z6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AA6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AB6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AC6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AD6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AE6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AF6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AG6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AH6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AI6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AJ6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AK6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AL6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AM6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AN6" t="n">
-        <v>55.82020768819547</v>
+        <v>52.58790871211168</v>
       </c>
       <c r="AO6" t="n">
-        <v>55.3099974766494</v>
+        <v>52.10632529784495</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12.80%</t>
+          <t>12.06%</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>13.97%</t>
+          <t>13.16%</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>16.30%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AL7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AM7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AN7" t="inlineStr">
         <is>
-          <t>16.29%</t>
+          <t>15.35%</t>
         </is>
       </c>
       <c r="AO7" t="inlineStr">
         <is>
-          <t>16.14%</t>
+          <t>15.21%</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kuwait Hospital</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="C8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="D8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="E8" t="n">
+        <v>34.20362646939189</v>
+      </c>
+      <c r="F8" t="n">
+        <v>33.43570421613532</v>
+      </c>
+      <c r="G8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="H8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="I8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="J8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="K8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="L8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="M8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="N8" t="n">
+        <v>31.90040593193773</v>
+      </c>
+      <c r="O8" t="n">
+        <v>31.8999017267234</v>
+      </c>
+      <c r="P8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="R8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="S8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="T8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="U8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="V8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="W8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="X8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>31.89985970962221</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>31.9983263636145</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>9.98%</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>9.76%</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="X9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AB9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AD9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AE9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AF9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AH9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AI9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AJ9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AK9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AL9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AM9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AN9" t="inlineStr">
+        <is>
+          <t>9.31%</t>
+        </is>
+      </c>
+      <c r="AO9" t="inlineStr">
+        <is>
+          <t>9.34%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Nasser Hospital</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="C10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="D10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="E10" t="n">
+        <v>41.30732537971645</v>
+      </c>
+      <c r="F10" t="n">
+        <v>45.06253677787249</v>
+      </c>
+      <c r="G10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="H10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="I10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="J10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="K10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="L10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="M10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="N10" t="n">
+        <v>52.57274586987847</v>
+      </c>
+      <c r="O10" t="n">
+        <v>52.5729431353918</v>
+      </c>
+      <c r="P10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="R10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="S10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="T10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="U10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="V10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="W10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="X10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>52.57295957418457</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>52.09151631434151</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>12.06%</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>13.15%</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AB11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AD11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AE11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AF11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AH11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AI11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AJ11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AK11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AL11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AM11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AN11" t="inlineStr">
+        <is>
+          <t>15.34%</t>
+        </is>
+      </c>
+      <c r="AO11" t="inlineStr">
+        <is>
+          <t>15.20%</t>
         </is>
       </c>
     </row>

</xml_diff>